<commit_message>
have issue in the system storing the vehicles in the excel using openpyxl and pandas going to learn and would fix this afterwards
</commit_message>
<xml_diff>
--- a/05 Smart Parking System/parking_lot.xlsx
+++ b/05 Smart Parking System/parking_lot.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,74 +434,77 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>PLATE</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>color</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>model</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>owner</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>entry_time</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>ticket_id</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1234567890</t>
-        </is>
+      <c r="A2" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>second car</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>car</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>red</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Toyota</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>John Doe</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>1768577706.768456</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>1234567890-1305</t>
+      <c r="G2" t="n">
+        <v>1768578334.572511</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>second car-2602</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing the entry function
</commit_message>
<xml_diff>
--- a/05 Smart Parking System/parking_lot.xlsx
+++ b/05 Smart Parking System/parking_lot.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -648,6 +648,76 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>car</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>red</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Toyota</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>John Doe</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>1768662257.194566</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1234567890-4601</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>test car</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>car</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>red</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Toyota</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>John Doe</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>1768662257.230299</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>test car-2789</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
starting making a text based rpg game in python and make class hero and dict of hero and monsters
</commit_message>
<xml_diff>
--- a/05 Smart Parking System/parking_lot.xlsx
+++ b/05 Smart Parking System/parking_lot.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,6 +468,76 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1345</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>car</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>aditya</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1768836913.170677</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1345-2566</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1111</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>car</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>aditya</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1768837051.922675</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1111-1933</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>